<commit_message>
Alt sat til nul i Excel arket
</commit_message>
<xml_diff>
--- a/assets/Gantt-projektplanlægger1.xlsx
+++ b/assets/Gantt-projektplanlægger1.xlsx
@@ -1050,8 +1050,8 @@
   </sheetPr>
   <dimension ref="B1:BO30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1382,7 +1382,7 @@
         <v>0</v>
       </c>
       <c r="G5" s="8">
-        <v>0.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -1402,7 +1402,7 @@
         <v>0</v>
       </c>
       <c r="G6" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -1422,7 +1422,7 @@
         <v>0</v>
       </c>
       <c r="G7" s="8">
-        <v>0.35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -1442,7 +1442,7 @@
         <v>0</v>
       </c>
       <c r="G8" s="8">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -1462,7 +1462,7 @@
         <v>0</v>
       </c>
       <c r="G9" s="8">
-        <v>0.85</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -1482,7 +1482,7 @@
         <v>0</v>
       </c>
       <c r="G10" s="8">
-        <v>0.85</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -1502,7 +1502,7 @@
         <v>0</v>
       </c>
       <c r="G11" s="8">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -1522,7 +1522,7 @@
         <v>0</v>
       </c>
       <c r="G12" s="8">
-        <v>0.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -1542,7 +1542,7 @@
         <v>0</v>
       </c>
       <c r="G13" s="8">
-        <v>0.75</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -1562,7 +1562,7 @@
         <v>0</v>
       </c>
       <c r="G14" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -1582,7 +1582,7 @@
         <v>0</v>
       </c>
       <c r="G15" s="8">
-        <v>0.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -1622,7 +1622,7 @@
         <v>0</v>
       </c>
       <c r="G17" s="8">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -1662,7 +1662,7 @@
         <v>0</v>
       </c>
       <c r="G19" s="8">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -1682,7 +1682,7 @@
         <v>0</v>
       </c>
       <c r="G20" s="8">
-        <v>0.8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -1782,7 +1782,7 @@
         <v>0</v>
       </c>
       <c r="G25" s="8">
-        <v>0.44</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -1822,7 +1822,7 @@
         <v>0</v>
       </c>
       <c r="G27" s="8">
-        <v>0.12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -1842,7 +1842,7 @@
         <v>0</v>
       </c>
       <c r="G28" s="8">
-        <v>0.05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -1882,7 +1882,7 @@
         <v>0</v>
       </c>
       <c r="G30" s="8">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Excel klar til lort
</commit_message>
<xml_diff>
--- a/assets/Gantt-projektplanlægger1.xlsx
+++ b/assets/Gantt-projektplanlægger1.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Projektplanlægger</t>
   </si>
@@ -45,9 +45,6 @@
   </si>
   <si>
     <t>AKTIVITET</t>
-  </si>
-  <si>
-    <t>Aktivitet 01</t>
   </si>
   <si>
     <t>Aktivitet 02</t>
@@ -232,12 +229,18 @@
   <si>
     <t>Aktivitet 08</t>
   </si>
+  <si>
+    <t>Hver kolonne svarer til 1 time</t>
+  </si>
+  <si>
+    <t>Benny Koder Headeren</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.24994659260841701"/>
@@ -336,6 +339,21 @@
       <name val="Corbel"/>
       <family val="2"/>
       <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1" tint="0.24994659260841701"/>
+      <name val="Corbel"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="1" tint="0.24994659260841701"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -524,7 +542,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -638,6 +656,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1051,13 +1075,13 @@
   <dimension ref="B1:BO30"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="2.6640625" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="37.44140625" style="2" customWidth="1"/>
     <col min="3" max="6" width="11.6640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="21" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="10" width="2.77734375" style="1"/>
@@ -1076,6 +1100,9 @@
       <c r="E1" s="13"/>
       <c r="F1" s="13"/>
       <c r="G1" s="13"/>
+      <c r="P1" s="38" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="24" t="s">
@@ -1086,14 +1113,14 @@
       <c r="E2" s="24"/>
       <c r="F2" s="24"/>
       <c r="G2" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H2" s="15">
         <v>1</v>
       </c>
       <c r="J2" s="16"/>
       <c r="K2" s="30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L2" s="31"/>
       <c r="M2" s="31"/>
@@ -1101,21 +1128,21 @@
       <c r="O2" s="32"/>
       <c r="P2" s="17"/>
       <c r="Q2" s="30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="R2" s="33"/>
       <c r="S2" s="33"/>
       <c r="T2" s="32"/>
       <c r="U2" s="18"/>
       <c r="V2" s="22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="W2" s="23"/>
       <c r="X2" s="23"/>
       <c r="Y2" s="34"/>
       <c r="Z2" s="19"/>
       <c r="AA2" s="35" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AB2" s="36"/>
       <c r="AC2" s="36"/>
@@ -1125,7 +1152,7 @@
       <c r="AG2" s="37"/>
       <c r="AH2" s="20"/>
       <c r="AI2" s="22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AJ2" s="23"/>
       <c r="AK2" s="23"/>
@@ -1140,22 +1167,22 @@
         <v>2</v>
       </c>
       <c r="C3" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="E3" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="F3" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="27" t="s">
-        <v>31</v>
-      </c>
       <c r="G3" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" s="21" t="s">
         <v>33</v>
-      </c>
-      <c r="H3" s="21" t="s">
-        <v>34</v>
       </c>
       <c r="I3" s="10"/>
       <c r="J3" s="11"/>
@@ -1163,7 +1190,7 @@
       <c r="L3" s="11"/>
       <c r="M3" s="11"/>
       <c r="N3" s="11"/>
-      <c r="O3" s="11"/>
+      <c r="O3" s="38"/>
       <c r="P3" s="11"/>
       <c r="Q3" s="11"/>
       <c r="R3" s="11"/>
@@ -1366,8 +1393,8 @@
       </c>
     </row>
     <row r="5" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="6" t="s">
-        <v>3</v>
+      <c r="B5" s="39" t="s">
+        <v>41</v>
       </c>
       <c r="C5" s="7">
         <v>0</v>
@@ -1387,7 +1414,7 @@
     </row>
     <row r="6" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6" s="7">
         <v>0</v>
@@ -1407,7 +1434,7 @@
     </row>
     <row r="7" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7" s="7">
         <v>0</v>
@@ -1427,7 +1454,7 @@
     </row>
     <row r="8" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" s="7">
         <v>0</v>
@@ -1447,7 +1474,7 @@
     </row>
     <row r="9" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" s="7">
         <v>0</v>
@@ -1467,7 +1494,7 @@
     </row>
     <row r="10" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10" s="7">
         <v>0</v>
@@ -1487,7 +1514,7 @@
     </row>
     <row r="11" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C11" s="7">
         <v>0</v>
@@ -1507,7 +1534,7 @@
     </row>
     <row r="12" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C12" s="7">
         <v>0</v>
@@ -1527,7 +1554,7 @@
     </row>
     <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C13" s="7">
         <v>0</v>
@@ -1547,7 +1574,7 @@
     </row>
     <row r="14" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C14" s="7">
         <v>0</v>
@@ -1567,7 +1594,7 @@
     </row>
     <row r="15" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C15" s="9">
         <v>0</v>
@@ -1587,7 +1614,7 @@
     </row>
     <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C16" s="7">
         <v>0</v>
@@ -1607,7 +1634,7 @@
     </row>
     <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C17" s="7">
         <v>0</v>
@@ -1627,7 +1654,7 @@
     </row>
     <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C18" s="7">
         <v>0</v>
@@ -1647,7 +1674,7 @@
     </row>
     <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C19" s="7">
         <v>0</v>
@@ -1667,7 +1694,7 @@
     </row>
     <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C20" s="7">
         <v>0</v>
@@ -1687,7 +1714,7 @@
     </row>
     <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B21" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C21" s="7">
         <v>0</v>
@@ -1707,7 +1734,7 @@
     </row>
     <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B22" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C22" s="7">
         <v>0</v>
@@ -1727,7 +1754,7 @@
     </row>
     <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B23" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C23" s="7">
         <v>0</v>
@@ -1747,7 +1774,7 @@
     </row>
     <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B24" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C24" s="7">
         <v>0</v>
@@ -1767,7 +1794,7 @@
     </row>
     <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B25" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C25" s="7">
         <v>0</v>
@@ -1787,7 +1814,7 @@
     </row>
     <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B26" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C26" s="7">
         <v>0</v>
@@ -1807,7 +1834,7 @@
     </row>
     <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B27" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C27" s="7">
         <v>0</v>
@@ -1827,7 +1854,7 @@
     </row>
     <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B28" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C28" s="7">
         <v>0</v>
@@ -1847,7 +1874,7 @@
     </row>
     <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B29" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C29" s="7">
         <v>0</v>
@@ -1867,7 +1894,7 @@
     </row>
     <row r="30" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B30" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C30" s="7">
         <v>0</v>

</xml_diff>